<commit_message>
Plano de ação e um pouco de css
</commit_message>
<xml_diff>
--- a/documentação/plano de ação.xlsx
+++ b/documentação/plano de ação.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefany\Documents\Projeto\Projeto2.0\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D553199-932C-4EA2-AE43-DE6FB03BFA34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70EA059-EF39-47B0-9CB6-68D8AC875B97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C89AAC5F-72A4-497C-9D3F-38DBA35842A6}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>Tarefa</t>
   </si>
@@ -59,28 +59,55 @@
     <t>Plano de Ação do Projeto Lixeira Inteligente</t>
   </si>
   <si>
-    <t>Tarefa 1</t>
-  </si>
-  <si>
-    <t>Tarefa 2</t>
-  </si>
-  <si>
-    <t>Tarefa 3</t>
-  </si>
-  <si>
-    <t>Tarefa 4</t>
-  </si>
-  <si>
-    <t>Tarefa 5</t>
-  </si>
-  <si>
-    <t>Tarefa 6</t>
-  </si>
-  <si>
-    <t>Tarefa 7</t>
-  </si>
-  <si>
-    <t>Tarefa 8</t>
+    <t>Tarefa 2-Site Estático Dashboard (Google Charts)</t>
+  </si>
+  <si>
+    <t>Tarefa 3-Site Estático Institucional - Local</t>
+  </si>
+  <si>
+    <t>Tarefa 4-Planilha de BackLog / Planilha de Sprints</t>
+  </si>
+  <si>
+    <t>Tarefa 7- Tabelas criadas no Azure</t>
+  </si>
+  <si>
+    <t>Tarefa 8-Teste Integrado (Arduino+DB) + API local com Node.JS</t>
+  </si>
+  <si>
+    <t>Tarefa 6- Diagrama de Arquitetura Local (Arduíno)</t>
+  </si>
+  <si>
+    <t>Tarefa 5-Especificação do Analytics</t>
+  </si>
+  <si>
+    <t>Tarefa 1 - Conferir Documentação</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Não iniciada</t>
+  </si>
+  <si>
+    <t>Em andamento</t>
+  </si>
+  <si>
+    <t>Todos</t>
+  </si>
+  <si>
+    <t>Product owner</t>
+  </si>
+  <si>
+    <t>Rafael/Stefany</t>
+  </si>
+  <si>
+    <t>Yuri/Graziela</t>
+  </si>
+  <si>
+    <t>Bruno/Gabreil</t>
   </si>
 </sst>
 </file>
@@ -205,9 +232,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -217,12 +250,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,138 +569,206 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="57.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="7">
+        <v>43929</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0.9</v>
+      </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0</v>
+      </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0.3</v>
+      </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="7">
+        <v>43929</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0.9</v>
+      </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0</v>
+      </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0</v>
+      </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0</v>
+      </c>
       <c r="G10" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deletado (documento de mvv) e sensores, teve uma modificação no plano de ação.
</commit_message>
<xml_diff>
--- a/documentação/plano de ação.xlsx
+++ b/documentação/plano de ação.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefany\Documents\Projeto\Projeto2.0\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70EA059-EF39-47B0-9CB6-68D8AC875B97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A445DEAC-A40D-4021-8456-06041C3EF11F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C89AAC5F-72A4-497C-9D3F-38DBA35842A6}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>Tarefa</t>
   </si>
@@ -56,9 +56,6 @@
     <t xml:space="preserve">Anotações </t>
   </si>
   <si>
-    <t>Plano de Ação do Projeto Lixeira Inteligente</t>
-  </si>
-  <si>
     <t>Tarefa 2-Site Estático Dashboard (Google Charts)</t>
   </si>
   <si>
@@ -92,9 +89,6 @@
     <t>Não iniciada</t>
   </si>
   <si>
-    <t>Em andamento</t>
-  </si>
-  <si>
     <t>Todos</t>
   </si>
   <si>
@@ -107,7 +101,13 @@
     <t>Yuri/Graziela</t>
   </si>
   <si>
-    <t>Bruno/Gabreil</t>
+    <t>Bruno/Gabriel</t>
+  </si>
+  <si>
+    <t>Plano de Ação do Projeto Smart trash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concluído </t>
   </si>
 </sst>
 </file>
@@ -241,6 +241,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -250,8 +252,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,7 +569,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,15 +584,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="6"/>
+      <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -619,155 +619,169 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="4">
+        <v>43929</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="7">
-        <v>43929</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0.9</v>
+      <c r="F3" s="5">
+        <v>1</v>
       </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="4">
+        <v>43952</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="8">
-        <v>0</v>
+      <c r="F4" s="5">
+        <v>1</v>
       </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="D5" s="4">
+        <v>43952</v>
+      </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="8">
-        <v>0.3</v>
+        <v>20</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="4">
+        <v>43952</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="7">
-        <v>43929</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="8">
-        <v>0.9</v>
+      <c r="F6" s="5">
+        <v>1</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="4">
+        <v>43953</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="8">
+      <c r="F7" s="5">
         <v>0</v>
       </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="D8" s="4">
+        <v>43954</v>
+      </c>
       <c r="E8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="8">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
       </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="D9" s="4">
+        <v>43955</v>
+      </c>
       <c r="E9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="8">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1</v>
       </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="4">
+        <v>43956</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="8">
-        <v>0</v>
+      <c r="F10" s="5">
+        <v>1</v>
       </c>
       <c r="G10" s="1"/>
     </row>

</xml_diff>